<commit_message>
Tilføjet de sidste instruktioner :eggplant: :sweat_drops:
</commit_message>
<xml_diff>
--- a/Instructions typer.xlsx
+++ b/Instructions typer.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tilfr\Dropbox\DTU\Computer arkitektur\Risky-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4A76E74-1B67-422B-BB6B-65176307418E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{021DF7CF-12CD-446A-8125-380FF335ED8E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8532" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diagram1" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="61">
   <si>
     <t>Instructions:</t>
   </si>
@@ -185,12 +185,36 @@
   </si>
   <si>
     <t>ECALL</t>
+  </si>
+  <si>
+    <t>MUL</t>
+  </si>
+  <si>
+    <t>MULH</t>
+  </si>
+  <si>
+    <t>MULHSU</t>
+  </si>
+  <si>
+    <t>MULHU</t>
+  </si>
+  <si>
+    <t>DIV</t>
+  </si>
+  <si>
+    <t>DIVU</t>
+  </si>
+  <si>
+    <t>REM</t>
+  </si>
+  <si>
+    <t>REMU</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -282,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -293,6 +317,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3302,7 +3327,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="84" workbookViewId="0" zoomToFit="1"/>
@@ -3641,11 +3666,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AI25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4306,6 +4331,142 @@
         <v>110011</v>
       </c>
     </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="1">
+        <v>110011</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="1">
+        <v>110011</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="1">
+        <v>10</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="1">
+        <v>110011</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="1">
+        <v>11</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="G21" s="1">
+        <v>110011</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="1">
+        <v>100</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="1">
+        <v>110011</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="1">
+        <v>101</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="1">
+        <v>110011</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="1">
+        <v>110</v>
+      </c>
+      <c r="F24" s="2"/>
+      <c r="G24" s="1">
+        <v>110011</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="1">
+        <v>111</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="1">
+        <v>110011</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>